<commit_message>
implement normal equation -> tested
</commit_message>
<xml_diff>
--- a/Dataset/Dataset_housing_prices_in_Portland.xlsx
+++ b/Dataset/Dataset_housing_prices_in_Portland.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CVS\Project\Learning_Machine_Learning\Dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CVS\Project\Machine_Learning\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EAC46201-7973-4024-983D-3C1382B3BC66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A9C721-7F02-4439-8CA7-3E9A0127636F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{0CC1F9A9-362C-4E67-8308-91D05C3CD422}"/>
+    <workbookView xWindow="-20610" yWindow="2205" windowWidth="20730" windowHeight="11310" xr2:uid="{0CC1F9A9-362C-4E67-8308-91D05C3CD422}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -425,14 +425,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2983F8C8-A6F5-457C-8AD3-11614AD224F2}">
   <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>